<commit_message>
Web Developement Angela Yu Section 12 update
</commit_message>
<xml_diff>
--- a/Web Developement/The Complete 2020 Web Development Bootcamp/The Complete 2020 Web Development Bootcamp.xlsx
+++ b/Web Developement/The Complete 2020 Web Development Bootcamp/The Complete 2020 Web Development Bootcamp.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\LENOVO\Desktop\Learning Essentials\Web Developement\The Complete 2020 Web Development Bootcamp\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A869B2DF-845D-443F-A653-57D462FA4BE6}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B74C41C4-7351-4590-A3F0-DC5B90854DF6}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -156,7 +156,7 @@
     <t>Time</t>
   </si>
   <si>
-    <t>Check if https://subhro2606.github.io/cv/ is working</t>
+    <t>Refer each time you create a new Website</t>
   </si>
 </sst>
 </file>
@@ -508,8 +508,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:I35"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F16" sqref="F16"/>
+    <sheetView tabSelected="1" topLeftCell="A8" workbookViewId="0">
+      <selection activeCell="C25" sqref="C25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -607,9 +607,7 @@
       <c r="F4" s="2"/>
       <c r="G4" s="2"/>
       <c r="H4" s="2"/>
-      <c r="I4" s="2" t="s">
-        <v>43</v>
-      </c>
+      <c r="I4" s="2"/>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A5" s="2" t="s">
@@ -618,7 +616,9 @@
       <c r="B5" s="3">
         <v>44055</v>
       </c>
-      <c r="C5" s="2"/>
+      <c r="C5" s="3">
+        <v>44055</v>
+      </c>
       <c r="D5" s="4">
         <v>4.3750000000000004E-2</v>
       </c>
@@ -635,7 +635,9 @@
       <c r="B6" s="3">
         <v>44055</v>
       </c>
-      <c r="C6" s="2"/>
+      <c r="C6" s="3">
+        <v>44055</v>
+      </c>
       <c r="D6" s="4">
         <v>0.12152777777777778</v>
       </c>
@@ -652,7 +654,9 @@
       <c r="B7" s="3">
         <v>44056</v>
       </c>
-      <c r="C7" s="2"/>
+      <c r="C7" s="3">
+        <v>44056</v>
+      </c>
       <c r="D7" s="4">
         <v>0.1076388888888889</v>
       </c>
@@ -669,7 +673,9 @@
       <c r="B8" s="3">
         <v>44056</v>
       </c>
-      <c r="C8" s="2"/>
+      <c r="C8" s="3">
+        <v>44057</v>
+      </c>
       <c r="D8" s="4">
         <v>0.1076388888888889</v>
       </c>
@@ -686,7 +692,9 @@
       <c r="B9" s="3">
         <v>44056</v>
       </c>
-      <c r="C9" s="2"/>
+      <c r="C9" s="3">
+        <v>44057</v>
+      </c>
       <c r="D9" s="4">
         <v>4.5833333333333337E-2</v>
       </c>
@@ -694,7 +702,9 @@
       <c r="F9" s="2"/>
       <c r="G9" s="2"/>
       <c r="H9" s="2"/>
-      <c r="I9" s="2"/>
+      <c r="I9" s="2" t="s">
+        <v>43</v>
+      </c>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A10" s="2" t="s">
@@ -703,7 +713,9 @@
       <c r="B10" s="3">
         <v>44057</v>
       </c>
-      <c r="C10" s="2"/>
+      <c r="C10" s="3">
+        <v>44062</v>
+      </c>
       <c r="D10" s="4">
         <v>0.10277777777777779</v>
       </c>
@@ -720,7 +732,9 @@
       <c r="B11" s="3">
         <v>44057</v>
       </c>
-      <c r="C11" s="2"/>
+      <c r="C11" s="3">
+        <v>44062</v>
+      </c>
       <c r="D11" s="4">
         <v>6.25E-2</v>
       </c>
@@ -737,7 +751,9 @@
       <c r="B12" s="3">
         <v>44057</v>
       </c>
-      <c r="C12" s="2"/>
+      <c r="C12" s="3">
+        <v>44062</v>
+      </c>
       <c r="D12" s="4">
         <v>3.9583333333333331E-2</v>
       </c>
@@ -754,7 +770,9 @@
       <c r="B13" s="3">
         <v>44057</v>
       </c>
-      <c r="C13" s="2"/>
+      <c r="C13" s="3">
+        <v>44062</v>
+      </c>
       <c r="D13" s="4">
         <v>1.3888888888888888E-2</v>
       </c>

</xml_diff>

<commit_message>
Web Developement Angela Yu Section 15 update
</commit_message>
<xml_diff>
--- a/Web Developement/The Complete 2020 Web Development Bootcamp/The Complete 2020 Web Development Bootcamp.xlsx
+++ b/Web Developement/The Complete 2020 Web Development Bootcamp/The Complete 2020 Web Development Bootcamp.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\LENOVO\Desktop\Learning Essentials\Web Developement\The Complete 2020 Web Development Bootcamp\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B74C41C4-7351-4590-A3F0-DC5B90854DF6}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DDA4352C-4DFE-4356-95D6-29CFB539A633}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -508,8 +508,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:I35"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A8" workbookViewId="0">
-      <selection activeCell="C25" sqref="C25"/>
+    <sheetView tabSelected="1" topLeftCell="A9" workbookViewId="0">
+      <selection activeCell="C18" sqref="C18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -789,7 +789,9 @@
       <c r="B14" s="3">
         <v>44061</v>
       </c>
-      <c r="C14" s="2"/>
+      <c r="C14" s="3">
+        <v>44063</v>
+      </c>
       <c r="D14" s="4">
         <v>6.5972222222222224E-2</v>
       </c>
@@ -806,7 +808,9 @@
       <c r="B15" s="3">
         <v>44061</v>
       </c>
-      <c r="C15" s="2"/>
+      <c r="C15" s="3">
+        <v>44063</v>
+      </c>
       <c r="D15" s="4">
         <v>3.6805555555555557E-2</v>
       </c>
@@ -823,7 +827,9 @@
       <c r="B16" s="3">
         <v>44061</v>
       </c>
-      <c r="C16" s="2"/>
+      <c r="C16" s="3">
+        <v>44063</v>
+      </c>
       <c r="D16" s="4">
         <v>1.0416666666666666E-2</v>
       </c>
@@ -840,7 +846,9 @@
       <c r="B17" s="3">
         <v>44061</v>
       </c>
-      <c r="C17" s="2"/>
+      <c r="C17" s="3">
+        <v>44063</v>
+      </c>
       <c r="D17" s="4">
         <v>2.4305555555555556E-2</v>
       </c>
@@ -857,7 +865,9 @@
       <c r="B18" s="3">
         <v>44061</v>
       </c>
-      <c r="C18" s="2"/>
+      <c r="C18" s="3">
+        <v>44063</v>
+      </c>
       <c r="D18" s="4">
         <v>5.5555555555555558E-3</v>
       </c>
@@ -872,7 +882,7 @@
         <v>23</v>
       </c>
       <c r="B19" s="3">
-        <v>44061</v>
+        <v>44063</v>
       </c>
       <c r="C19" s="2"/>
       <c r="D19" s="4">
@@ -889,7 +899,7 @@
         <v>24</v>
       </c>
       <c r="B20" s="3">
-        <v>44061</v>
+        <v>44063</v>
       </c>
       <c r="C20" s="2"/>
       <c r="D20" s="4">
@@ -906,7 +916,7 @@
         <v>25</v>
       </c>
       <c r="B21" s="3">
-        <v>44062</v>
+        <v>44063</v>
       </c>
       <c r="C21" s="2"/>
       <c r="D21" s="4">
@@ -923,7 +933,7 @@
         <v>26</v>
       </c>
       <c r="B22" s="3">
-        <v>44062</v>
+        <v>44064</v>
       </c>
       <c r="C22" s="2"/>
       <c r="D22" s="4">
@@ -940,7 +950,7 @@
         <v>27</v>
       </c>
       <c r="B23" s="3">
-        <v>44062</v>
+        <v>44064</v>
       </c>
       <c r="C23" s="2"/>
       <c r="D23" s="4">
@@ -957,7 +967,7 @@
         <v>28</v>
       </c>
       <c r="B24" s="3">
-        <v>44063</v>
+        <v>44064</v>
       </c>
       <c r="C24" s="2"/>
       <c r="D24" s="4">
@@ -974,7 +984,7 @@
         <v>29</v>
       </c>
       <c r="B25" s="3">
-        <v>44063</v>
+        <v>44064</v>
       </c>
       <c r="C25" s="2"/>
       <c r="D25" s="4">
@@ -991,7 +1001,7 @@
         <v>30</v>
       </c>
       <c r="B26" s="3">
-        <v>44063</v>
+        <v>44064</v>
       </c>
       <c r="C26" s="2"/>
       <c r="D26" s="4">
@@ -1008,7 +1018,7 @@
         <v>31</v>
       </c>
       <c r="B27" s="3">
-        <v>44063</v>
+        <v>44065</v>
       </c>
       <c r="C27" s="2"/>
       <c r="D27" s="4">
@@ -1025,7 +1035,7 @@
         <v>32</v>
       </c>
       <c r="B28" s="3">
-        <v>44064</v>
+        <v>44065</v>
       </c>
       <c r="C28" s="2"/>
       <c r="D28" s="4">
@@ -1042,7 +1052,7 @@
         <v>33</v>
       </c>
       <c r="B29" s="3">
-        <v>44064</v>
+        <v>44065</v>
       </c>
       <c r="C29" s="2"/>
       <c r="D29" s="4">
@@ -1059,7 +1069,7 @@
         <v>34</v>
       </c>
       <c r="B30" s="3">
-        <v>44064</v>
+        <v>44065</v>
       </c>
       <c r="C30" s="2"/>
       <c r="D30" s="4">
@@ -1076,7 +1086,7 @@
         <v>35</v>
       </c>
       <c r="B31" s="3">
-        <v>44064</v>
+        <v>44066</v>
       </c>
       <c r="C31" s="2"/>
       <c r="D31" s="4">
@@ -1093,7 +1103,7 @@
         <v>36</v>
       </c>
       <c r="B32" s="3">
-        <v>44065</v>
+        <v>44066</v>
       </c>
       <c r="C32" s="2"/>
       <c r="D32" s="4">
@@ -1110,7 +1120,7 @@
         <v>37</v>
       </c>
       <c r="B33" s="3">
-        <v>44065</v>
+        <v>44067</v>
       </c>
       <c r="C33" s="2"/>
       <c r="D33" s="4">
@@ -1127,7 +1137,7 @@
         <v>38</v>
       </c>
       <c r="B34" s="3">
-        <v>44065</v>
+        <v>44068</v>
       </c>
       <c r="C34" s="2"/>
       <c r="D34" s="4">
@@ -1144,7 +1154,7 @@
         <v>39</v>
       </c>
       <c r="B35" s="3">
-        <v>44066</v>
+        <v>44069</v>
       </c>
       <c r="C35" s="2"/>
       <c r="D35" s="4">

</xml_diff>

<commit_message>
express & git tutorial complete
</commit_message>
<xml_diff>
--- a/Web Developement/The Complete 2020 Web Development Bootcamp/The Complete 2020 Web Development Bootcamp.xlsx
+++ b/Web Developement/The Complete 2020 Web Development Bootcamp/The Complete 2020 Web Development Bootcamp.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\LENOVO\Desktop\Learning Essentials\Web Developement\The Complete 2020 Web Development Bootcamp\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DDA4352C-4DFE-4356-95D6-29CFB539A633}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9F77D9C2-3C3C-410D-A447-CB994DD39C45}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -508,8 +508,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:I35"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A9" workbookViewId="0">
-      <selection activeCell="C18" sqref="C18"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B24" sqref="B23:B24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -884,7 +884,9 @@
       <c r="B19" s="3">
         <v>44063</v>
       </c>
-      <c r="C19" s="2"/>
+      <c r="C19" s="3">
+        <v>44064</v>
+      </c>
       <c r="D19" s="4">
         <v>2.7083333333333334E-2</v>
       </c>
@@ -901,7 +903,9 @@
       <c r="B20" s="3">
         <v>44063</v>
       </c>
-      <c r="C20" s="2"/>
+      <c r="C20" s="3">
+        <v>44064</v>
+      </c>
       <c r="D20" s="4">
         <v>5.1388888888888894E-2</v>
       </c>

</xml_diff>